<commit_message>
Update vault by sv
</commit_message>
<xml_diff>
--- a/fnz/ausgaben.xlsx
+++ b/fnz/ausgaben.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="204">
   <si>
     <t xml:space="preserve">Kostenstelle</t>
   </si>
@@ -439,6 +439,12 @@
   </si>
   <si>
     <t xml:space="preserve">15.05.204</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reiseversicherung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Erogo</t>
   </si>
   <si>
     <t xml:space="preserve">Produkt</t>
@@ -1016,8 +1022,8 @@
   </sheetPr>
   <dimension ref="A1:AC1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A62" activeCellId="0" sqref="A62"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G62" activeCellId="0" sqref="G62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2251,9 +2257,22 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E62" s="7"/>
-      <c r="F62" s="8"/>
-      <c r="G62" s="9"/>
+      <c r="B62" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E62" s="7" t="n">
+        <f aca="false">24/12</f>
+        <v>2</v>
+      </c>
+      <c r="F62" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="G62" s="9" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E63" s="7"/>
@@ -6948,7 +6967,7 @@
   <dimension ref="A1:AA3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="G62 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6961,22 +6980,22 @@
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2"/>
       <c r="B1" s="2" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
@@ -7002,13 +7021,13 @@
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6"/>
       <c r="B2" s="6" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7016,22 +7035,22 @@
         <v>26</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C3" s="6" t="n">
         <v>201139069</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F3" s="6" t="n">
         <v>842</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -7053,7 +7072,7 @@
   <dimension ref="A1:D1001"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J31" activeCellId="0" sqref="J31"/>
+      <selection pane="topLeft" activeCell="J31" activeCellId="1" sqref="G62 J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7065,21 +7084,21 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C2" s="17" t="n">
         <v>15000</v>
@@ -7091,10 +7110,10 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C3" s="17" t="n">
         <v>5000</v>
@@ -7106,10 +7125,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C4" s="17" t="n">
         <v>5000</v>
@@ -7121,10 +7140,10 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C5" s="17" t="n">
         <v>5000</v>
@@ -7136,10 +7155,10 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C6" s="17" t="n">
         <v>5000</v>
@@ -7151,10 +7170,10 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C7" s="17" t="n">
         <v>5000</v>
@@ -7166,10 +7185,10 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>164</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>162</v>
       </c>
       <c r="C8" s="17" t="n">
         <v>5000</v>
@@ -7182,7 +7201,7 @@
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="24"/>
       <c r="B9" s="6" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C9" s="17"/>
       <c r="D9" s="25" t="n">
@@ -11177,7 +11196,7 @@
   <dimension ref="A1:Y1001"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="G62 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11188,22 +11207,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="E1" s="26" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="G1" s="10"/>
       <c r="H1" s="10"/>
@@ -11881,7 +11900,7 @@
         <v>190</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11903,7 +11922,7 @@
         <v>181</v>
       </c>
       <c r="F35" s="10" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11925,7 +11944,7 @@
         <v>150</v>
       </c>
       <c r="F36" s="10" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11947,7 +11966,7 @@
         <v>23</v>
       </c>
       <c r="F37" s="10" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11970,7 +11989,7 @@
         <v>136</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11993,7 +12012,7 @@
         <v>160</v>
       </c>
       <c r="F39" s="10" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12016,10 +12035,10 @@
         <v>160</v>
       </c>
       <c r="F40" s="10" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="K40" s="6" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="L40" s="27"/>
       <c r="M40" s="28"/>
@@ -12038,7 +12057,7 @@
       <c r="E41" s="28"/>
       <c r="F41" s="10"/>
       <c r="H41" s="6" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="I41" s="6" t="n">
         <v>1435.5</v>
@@ -12068,13 +12087,13 @@
         <v>40</v>
       </c>
       <c r="F42" s="10" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="G42" s="6" t="n">
         <v>1.19</v>
       </c>
       <c r="H42" s="6" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="I42" s="28" t="n">
         <f aca="false">SUM(E42:E1001)</f>
@@ -12106,13 +12125,13 @@
         <v>200</v>
       </c>
       <c r="F43" s="10" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="G43" s="6" t="n">
         <v>1.19</v>
       </c>
       <c r="H43" s="29" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="I43" s="30" t="n">
         <f aca="false">I41-I42</f>
@@ -12144,7 +12163,7 @@
         <v>154</v>
       </c>
       <c r="F44" s="10" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="G44" s="6" t="n">
         <v>1.16</v>
@@ -12171,7 +12190,7 @@
         <v>197</v>
       </c>
       <c r="F45" s="10" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="G45" s="6" t="n">
         <v>1.16</v>
@@ -12198,7 +12217,7 @@
         <v>181</v>
       </c>
       <c r="F46" s="10" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="G46" s="6" t="n">
         <v>1.16</v>
@@ -12223,7 +12242,7 @@
         <v>189</v>
       </c>
       <c r="F47" s="10" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="G47" s="6" t="n">
         <v>1.16</v>
@@ -12248,7 +12267,7 @@
         <v>194</v>
       </c>
       <c r="F48" s="10" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="G48" s="6" t="n">
         <v>1.16</v>
@@ -12273,7 +12292,7 @@
         <v>135</v>
       </c>
       <c r="F49" s="10" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="G49" s="6" t="n">
         <v>1.16</v>
@@ -12298,7 +12317,7 @@
         <v>190</v>
       </c>
       <c r="F50" s="10" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="G50" s="6" t="n">
         <v>1.19</v>
@@ -12403,7 +12422,7 @@
         <v>1.19</v>
       </c>
       <c r="I55" s="6" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18121,7 +18140,7 @@
   <dimension ref="A1:C1002"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
+      <selection pane="topLeft" activeCell="C24" activeCellId="1" sqref="G62 C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18133,7 +18152,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="31" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B1" s="32"/>
     </row>
@@ -18235,7 +18254,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B14" s="34" t="n">
         <f aca="false">AVERAGE(B2:B13)</f>
@@ -18249,7 +18268,7 @@
         <v>295.366666666667</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18258,7 +18277,7 @@
         <v>814.45</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18267,7 +18286,7 @@
         <v>145.21</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18276,7 +18295,7 @@
         <v>117.13</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18285,7 +18304,7 @@
         <v>292</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18294,7 +18313,7 @@
         <v>316.7</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18303,12 +18322,12 @@
         <v>715.85</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B22" s="34" t="n">
         <f aca="false">B14-SUM(B15:B21)</f>

</xml_diff>